<commit_message>
add to type to skki store, update, import
</commit_message>
<xml_diff>
--- a/public/templates/import_skki_template.xlsx
+++ b/public/templates/import_skki_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maul\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\monitoring-api\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6393D75-D149-4708-8471-2571E13E1DD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E26A8B-E912-4EC4-B1D8-0FEDF9723ADF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{40E8CDBE-C041-4AF3-8CAE-C0C1B20AB6A6}"/>
   </bookViews>
@@ -28,6 +28,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maul</author>
+    <author>Ichwan</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E3DD29C8-960D-49A1-AC7E-F5C377B5ED14}">
@@ -62,7 +63,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{8E606A50-3B72-4C4A-98DE-F5C9BFBA59F7}">
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{168B9084-5429-4408-A50D-303A4CA85762}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Wajib diisi
+MURNI
+LUNCURAN</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{8E606A50-3B72-4C4A-98DE-F5C9BFBA59F7}">
       <text>
         <r>
           <rPr>
@@ -82,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Nomor SKKI</t>
   </si>
@@ -109,6 +126,33 @@
   </si>
   <si>
     <t>2022.DDKI.5.002</t>
+  </si>
+  <si>
+    <t>WBSJ1</t>
+  </si>
+  <si>
+    <t>WBSJ2</t>
+  </si>
+  <si>
+    <t>WBSM1</t>
+  </si>
+  <si>
+    <t>WBSM2</t>
+  </si>
+  <si>
+    <t>Tipe</t>
+  </si>
+  <si>
+    <t>MURNI</t>
+  </si>
+  <si>
+    <t>LUNCURAN</t>
+  </si>
+  <si>
+    <t>PRKSKKI.2022.DDKI.5.001</t>
+  </si>
+  <si>
+    <t>PRKSKKI.2022.DDKI.5.002</t>
   </si>
 </sst>
 </file>
@@ -117,7 +161,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -157,27 +201,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -189,14 +218,17 @@
     <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -516,18 +548,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAAA200-6412-4E12-B322-CF7E891DADE0}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="6" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,37 +581,56 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="F2">
-        <v>3</v>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="F3">
-        <v>3</v>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>